<commit_message>
Testes de usuário adicionados
</commit_message>
<xml_diff>
--- a/DesafioAutomacaoAPIBase2/DataDriven/Serverest.xlsx
+++ b/DesafioAutomacaoAPIBase2/DataDriven/Serverest.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josias\source\repos\DesafioAutomacaoAPIRest_Dev\DesafioAutomacaoAPIBase2\DesafioAutomacaoAPIBase2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josias\source\repos\DesafioAutomacaoAPIBase2_DEV\DesafioAutomacaoAPIBase2\DataDriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492AA9F4-2A11-4E06-BFC4-F6AA9F68F5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E32C51E-A79E-424F-A4EA-3A2DAB6A1DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{6FC5C8F2-1EA8-4D1D-8AA2-8F2DF5FACFA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Produtos" sheetId="1" r:id="rId1"/>
-    <sheet name="ProdutoId" sheetId="2" r:id="rId2"/>
+    <sheet name="Usuarios" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>nome</t>
   </si>
@@ -113,17 +113,135 @@
     <t>Caixa de som PC Sound</t>
   </si>
   <si>
-    <t>produto_id</t>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>administrador</t>
+  </si>
+  <si>
+    <t>João Malcávio Felix</t>
+  </si>
+  <si>
+    <t>Abrantes Delcácio Júnior</t>
+  </si>
+  <si>
+    <t>Abadias Plentofídio de Souza</t>
+  </si>
+  <si>
+    <t>Joesley Primo Dias</t>
+  </si>
+  <si>
+    <t>Creuzedétio Marcos e Silva</t>
+  </si>
+  <si>
+    <t>Malaquias Filomeno</t>
+  </si>
+  <si>
+    <t>Olívia Antonietta Santos</t>
+  </si>
+  <si>
+    <t>Gertrudes Anancy Amâncio</t>
+  </si>
+  <si>
+    <t>Paulo Silva das Dores</t>
+  </si>
+  <si>
+    <t>Cipriano Vigílio Theodoro</t>
+  </si>
+  <si>
+    <t>jmfelix@yahoo.com.br</t>
+  </si>
+  <si>
+    <t>abdelc@hotmail.com.br</t>
+  </si>
+  <si>
+    <t>abaplesouza@uol.com.br</t>
+  </si>
+  <si>
+    <t>joesley_1987@hotmal.com</t>
+  </si>
+  <si>
+    <t>creuzedetio_silva@outlook.com</t>
+  </si>
+  <si>
+    <t>malaquias_filo@gmail.com.br</t>
+  </si>
+  <si>
+    <t>olivia_1234@bol.com.br</t>
+  </si>
+  <si>
+    <t>gertrudes1995@intelig.com.br</t>
+  </si>
+  <si>
+    <t>paulosilva_dores@ig.com.br</t>
+  </si>
+  <si>
+    <t>cipriano_theodoro@yahoo.com.br</t>
+  </si>
+  <si>
+    <t>adm123</t>
+  </si>
+  <si>
+    <t>adm124</t>
+  </si>
+  <si>
+    <t>adm125</t>
+  </si>
+  <si>
+    <t>adm126</t>
+  </si>
+  <si>
+    <t>adm127</t>
+  </si>
+  <si>
+    <t>adm128</t>
+  </si>
+  <si>
+    <t>adm129</t>
+  </si>
+  <si>
+    <t>adm130</t>
+  </si>
+  <si>
+    <t>adm131</t>
+  </si>
+  <si>
+    <t>adm132</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,13 +264,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -652,23 +774,189 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9AA7D6F-E6FB-46F6-9BE3-44A4B0ACFEC5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
       </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{6459A1F5-38BE-423B-B8CE-98FA6F8ED799}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{C32A1B37-D090-4B6E-8523-BAE46A36A0B4}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{B165D18A-1394-4B54-9F5B-B674A975095D}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{32674231-C92E-4736-AEF4-44FE84B01757}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{26BBE00A-2D9B-4B27-B49D-98D580FB353A}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{49660F01-A5CF-4922-9B23-92ED46AA51C8}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{9F0C4F0F-7FB8-4925-8ED5-0F1301FEE9D9}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{E0A2B826-FF5F-4FAA-AF77-A0CCD0945C58}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{EA32E163-9741-4FCC-AC64-068447906019}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{C6FCF48F-F69F-4711-884D-0604AB118BEC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>